<commit_message>
Built UI and made it as application
</commit_message>
<xml_diff>
--- a/data/Envizi_SetupConfig_1_INBank.xlsx
+++ b/data/Envizi_SetupConfig_1_INBank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gandhi/GandhiMain/700-Apps/envizi-location-service/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vidishalimbola/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968FF6D5-614F-0243-A5BC-566D21A6DD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB14099-A2D0-A241-A42A-E58BB680154E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29920" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>ORGANIZATION</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>G20-LS- Chennai DC</t>
+  </si>
+  <si>
+    <t>G20-LS- Gujarat DC</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
   </si>
 </sst>
 </file>
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -978,6 +984,34 @@
       <c r="O13"/>
       <c r="P13"/>
     </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14"/>
+      <c r="P14"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Q13" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>